<commit_message>
remark interpritation done / not integrated
</commit_message>
<xml_diff>
--- a/test_usgs/output_previous/output_1.xlsx
+++ b/test_usgs/output_previous/output_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Abrasives_raw_info"/>
@@ -4686,7 +4686,7 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7262,7 +7262,7 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>